<commit_message>
gráficos e filtragem por semana adicionados
</commit_message>
<xml_diff>
--- a/archive/planilha_sample.xlsx
+++ b/archive/planilha_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\SPIP2-Projeto-Extensao.edit\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E342FD-6671-4A41-BB12-47699E3F8398}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7EAFE4-4AD2-48F0-8EB2-F4AEEEC64190}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:AE1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1685,10 +1685,10 @@
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36">
-        <v>45208</v>
+        <v>45214</v>
       </c>
       <c r="B7" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>58</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36">
-        <v>45208</v>
+        <v>45215</v>
       </c>
       <c r="B8" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>59</v>
@@ -1789,10 +1789,10 @@
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
-        <v>45208</v>
+        <v>45216</v>
       </c>
       <c r="B9" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>54</v>
@@ -1843,10 +1843,10 @@
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36">
-        <v>45208</v>
+        <v>45217</v>
       </c>
       <c r="B10" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="52" t="s">
         <v>94</v>
@@ -1897,10 +1897,10 @@
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
-        <v>45208</v>
+        <v>45218</v>
       </c>
       <c r="B11" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>93</v>
@@ -1951,10 +1951,10 @@
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="B12" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="52" t="s">
         <v>97</v>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36">
-        <v>45209</v>
+        <v>45221</v>
       </c>
       <c r="B13" s="5">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>98</v>
@@ -2059,10 +2059,10 @@
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36">
-        <v>45209</v>
+        <v>45222</v>
       </c>
       <c r="B14" s="5">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="52" t="s">
         <v>102</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36">
-        <v>45209</v>
+        <v>45223</v>
       </c>
       <c r="B15" s="5">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" s="52" t="s">
         <v>95</v>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
-        <v>45209</v>
+        <v>45224</v>
       </c>
       <c r="B16" s="5">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" s="52" t="s">
         <v>99</v>
@@ -2237,10 +2237,10 @@
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
-        <v>45209</v>
+        <v>45225</v>
       </c>
       <c r="B17" s="5">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" s="52" t="s">
         <v>100</v>
@@ -2291,10 +2291,10 @@
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36">
-        <v>45210</v>
+        <v>45228</v>
       </c>
       <c r="B18" s="5">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>101</v>
@@ -2349,10 +2349,10 @@
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
-        <v>45210</v>
+        <v>45228</v>
       </c>
       <c r="B19" s="5">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C19" s="53" t="s">
         <v>96</v>

</xml_diff>